<commit_message>
updated to latest version of xw
</commit_message>
<xml_diff>
--- a/reporting_bigmac/bigmac_index.xlsx
+++ b/reporting_bigmac/bigmac_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/DEV/xlwings-demo/reporting_bigmac/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-demo\reporting_bigmac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C9623E-10BC-2548-816A-9C83A004C8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C17362-C926-46B8-8E6C-0A5C7696EB94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5140" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{EE5635DF-CB9B-554F-BBBB-4686181DBE0F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{EE5635DF-CB9B-554F-BBBB-4686181DBE0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>&lt;frame&gt;</t>
   </si>
@@ -121,9 +121,6 @@
     <t>import xlwings as xw</t>
   </si>
   <si>
-    <t>from xlwings.reports import create_report  # part of xlwings PRO</t>
-  </si>
-  <si>
     <t>def main():</t>
   </si>
   <si>
@@ -251,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">    url = os.path.join(os.path.dirname(template.fullname), 'big-mac-raw-index.csv')</t>
+  </si>
+  <si>
+    <t># Requires a license key: https://www.xlwings.org/trial</t>
+  </si>
+  <si>
+    <t>from xlwings.pro.reports import create_report</t>
   </si>
 </sst>
 </file>
@@ -1763,19 +1766,19 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="37.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="27.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="28.33203125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="18.1875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8125" style="2"/>
+    <col min="3" max="3" width="37.3125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.8125" style="2"/>
+    <col min="5" max="5" width="27.1875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.8125" style="2"/>
+    <col min="7" max="7" width="28.3125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="10.8125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="15" customFormat="1" ht="67" x14ac:dyDescent="0.95">
+    <row r="4" spans="1:7" s="15" customFormat="1" ht="65.650000000000006" x14ac:dyDescent="2.25">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
@@ -1794,7 +1797,7 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -1806,11 +1809,11 @@
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
@@ -1822,12 +1825,12 @@
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="18" t="s">
         <v>21</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -1847,11 +1850,11 @@
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
@@ -1863,11 +1866,11 @@
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="16"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="18" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -1887,25 +1890,25 @@
       <c r="F21" s="5"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G27" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="19" t="s">
         <v>21</v>
       </c>
@@ -1989,12 +1992,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>36617</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>36982</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>37347</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>37712</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>38108</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2060,132 +2063,132 @@
         <v>38504</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM7" s="17">
         <v>38718</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM8" s="17">
         <v>38838</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM9" s="17">
         <v>39083</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM10" s="17">
         <v>39234</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM11" s="17">
         <v>39600</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM12" s="17">
         <v>39995</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM13" s="17">
         <v>40179</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM14" s="17">
         <v>40360</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM15" s="17">
         <v>40725</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.5">
       <c r="AM16" s="17">
         <v>40909</v>
       </c>
     </row>
-    <row r="17" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM17" s="17">
         <v>41091</v>
       </c>
     </row>
-    <row r="18" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM18" s="17">
         <v>41275</v>
       </c>
     </row>
-    <row r="19" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM19" s="17">
         <v>41456</v>
       </c>
     </row>
-    <row r="20" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM20" s="17">
         <v>41640</v>
       </c>
     </row>
-    <row r="21" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM21" s="17">
         <v>41821</v>
       </c>
     </row>
-    <row r="22" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM22" s="17">
         <v>42005</v>
       </c>
     </row>
-    <row r="23" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM23" s="17">
         <v>42186</v>
       </c>
     </row>
-    <row r="24" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM24" s="17">
         <v>42370</v>
       </c>
     </row>
-    <row r="25" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM25" s="17">
         <v>42552</v>
       </c>
     </row>
-    <row r="26" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM26" s="17">
         <v>42736</v>
       </c>
     </row>
-    <row r="27" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM27" s="17">
         <v>42917</v>
       </c>
     </row>
-    <row r="28" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM28" s="17">
         <v>43101</v>
       </c>
     </row>
-    <row r="29" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM29" s="17">
         <v>43282</v>
       </c>
     </row>
-    <row r="30" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM30" s="17">
         <v>43466</v>
       </c>
     </row>
-    <row r="31" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM31" s="17">
         <v>43655</v>
       </c>
     </row>
-    <row r="32" spans="39:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="39:39" x14ac:dyDescent="0.5">
       <c r="AM32" s="17">
         <v>43844</v>
       </c>
@@ -2207,13 +2210,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -2236,249 +2239,254 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD21A84-70FD-C74F-8FF8-009CCC5FE883}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="134.1640625" style="20" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="21"/>
+    <col min="1" max="1" width="134.1875" style="20" customWidth="1"/>
+    <col min="2" max="16384" width="10.8125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A9" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A11" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A12" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A13" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A14" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A15" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A17" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A19" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A20" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A21" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A22" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A24" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A25" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A26" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A27" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A28" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A29" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A31" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A32" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A33" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A34" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A36" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A37" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A38" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A39" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A41" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A42" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A43" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A45" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A46" s="20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A47" s="20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A48" s="20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A49" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A51" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A52" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A53" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A54" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A55" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A56" s="20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A58" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A59" s="20" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to latest xlwings API
</commit_message>
<xml_diff>
--- a/reporting_bigmac/bigmac_index.xlsx
+++ b/reporting_bigmac/bigmac_index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-demo\reporting_bigmac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CB38EC-DE61-455A-A29C-2FC7B5AF8D54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76B26B8-E76A-42E6-81A3-3F86ECF47681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{EE5635DF-CB9B-554F-BBBB-4686181DBE0F}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>&lt;frame&gt;</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>from xlwings.pro.reports import create_report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wb.to_pdf(include=1)</t>
   </si>
 </sst>
 </file>
@@ -2239,9 +2242,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD21A84-70FD-C74F-8FF8-009CCC5FE883}">
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2489,8 +2494,13 @@
         <v>65</v>
       </c>
     </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A60" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>